<commit_message>
Updating presentation and examples for Week 03
</commit_message>
<xml_diff>
--- a/161702/presentation/02 - Review Divide and Conquer/Rod cutting illustration.xlsx
+++ b/161702/presentation/02 - Review Divide and Conquer/Rod cutting illustration.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>length</t>
   </si>
@@ -70,14 +70,70 @@
   </si>
   <si>
     <t>3, 10</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -407,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection sqref="A1:K2"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +472,8 @@
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="3.7109375" customWidth="1"/>
     <col min="8" max="8" width="5.5703125" customWidth="1"/>
-    <col min="9" max="11" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="10" max="11" width="3.7109375" customWidth="1"/>
     <col min="12" max="14" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.7109375" customWidth="1"/>
   </cols>
@@ -573,13 +630,13 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>
@@ -598,6 +655,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -605,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>